<commit_message>
re-run species script and prepare version of data base with unfinished pressure variable categorization
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Brown.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Brown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/estb_dtu_dk/Documents/Projects/SEAwise/T4.1/Data extraction/Read only SP files to be uploaded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D6C9C-2292-4C5A-9818-61026ACDB2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E6AF89A-9660-4FB2-B080-F6635101DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$36</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -2391,7 +2391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="388">
   <si>
     <t>SearchID</t>
   </si>
@@ -3548,9 +3548,6 @@
     <t>Time Series Analyses</t>
   </si>
   <si>
-    <t>size based indiators</t>
-  </si>
-  <si>
     <t>Fishing pressure as desired catch</t>
   </si>
   <si>
@@ -3584,9 +3581,6 @@
   </si>
   <si>
     <t>Discards generated</t>
-  </si>
-  <si>
-    <t>the power of the trawl survey to detect trends is generally poor.</t>
   </si>
 </sst>
 </file>
@@ -4066,25 +4060,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX34"/>
+  <dimension ref="A1:AX36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AQ12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AV16" sqref="AV16"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="13" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10" style="11" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" style="11" customWidth="1"/>
-    <col min="6" max="12" width="13" style="11" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.08984375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="7.08984375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="5.7265625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="7.90625" style="11" customWidth="1"/>
     <col min="13" max="13" width="4.6328125" style="11" customWidth="1"/>
     <col min="14" max="14" width="6" style="11" customWidth="1"/>
-    <col min="15" max="15" width="3.54296875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="6.7265625" style="11" customWidth="1"/>
     <col min="16" max="16" width="12.453125" style="11" customWidth="1"/>
     <col min="17" max="17" width="18.7265625" style="11" customWidth="1"/>
     <col min="18" max="18" width="13" style="11"/>
@@ -4413,7 +4413,7 @@
         <v>159</v>
       </c>
       <c r="AO3" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AQ3" s="11" t="s">
         <v>164</v>
@@ -6677,7 +6677,7 @@
         <v>160</v>
       </c>
       <c r="AO22" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AQ22" s="11" t="s">
         <v>164</v>
@@ -7295,40 +7295,40 @@
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E28" s="11">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="G28" s="11">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H28" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="11">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="J28" s="11">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="N28" s="11" t="s">
         <v>249</v>
@@ -7336,52 +7336,118 @@
       <c r="O28" s="11" t="s">
         <v>250</v>
       </c>
+      <c r="P28" s="11" t="s">
+        <v>287</v>
+      </c>
       <c r="Q28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="R28" s="11" t="s">
-        <v>84</v>
+      <c r="S28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="T28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="X28" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z28" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="AA28" s="11">
+        <v>3</v>
+      </c>
+      <c r="AB28" s="11">
+        <v>3</v>
+      </c>
+      <c r="AC28" s="11">
+        <v>3</v>
       </c>
       <c r="AF28" s="11">
         <v>4.4000000000000004</v>
       </c>
+      <c r="AG28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH28" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL28" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="AM28" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN28" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO28" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="AQ28" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AT28" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="AU28" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="AV28" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW28" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX28" s="11" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E29" s="11">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>278</v>
       </c>
       <c r="G29" s="11">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H29" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="11">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="J29" s="11">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="N29" s="11" t="s">
         <v>249</v>
@@ -7389,6 +7455,9 @@
       <c r="O29" s="11" t="s">
         <v>250</v>
       </c>
+      <c r="P29" s="11" t="s">
+        <v>287</v>
+      </c>
       <c r="Q29" s="11" t="s">
         <v>21</v>
       </c>
@@ -7438,7 +7507,7 @@
         <v>232</v>
       </c>
       <c r="AN29" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO29" s="11" t="s">
         <v>373</v>
@@ -7450,54 +7519,54 @@
         <v>372</v>
       </c>
       <c r="AU29" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AV29" s="11" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="AW29" s="11" t="s">
         <v>209</v>
       </c>
       <c r="AX29" s="11" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E30" s="11">
         <v>2004</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="G30" s="11">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H30" s="11">
         <v>1</v>
       </c>
       <c r="I30" s="11">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="J30" s="11">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="N30" s="11" t="s">
         <v>249</v>
@@ -7508,115 +7577,55 @@
       <c r="Q30" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S30" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="T30" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="U30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V30" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="W30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="X30" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z30" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="AA30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AB30" s="11">
-        <v>3</v>
-      </c>
-      <c r="AC30" s="11">
-        <v>3</v>
+      <c r="R30" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="AF30" s="11">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AG30" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH30" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL30" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="AM30" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN30" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO30" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="AQ30" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AT30" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="AU30" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="AV30" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="AW30" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX30" s="11" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E31" s="11">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="G31" s="11">
-        <v>503</v>
+        <v>61</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1</v>
       </c>
       <c r="I31" s="11">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="J31" s="11">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="N31" s="11" t="s">
         <v>249</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>305</v>
+        <v>250</v>
       </c>
       <c r="Q31" s="11" t="s">
         <v>21</v>
@@ -7625,42 +7634,45 @@
         <v>84</v>
       </c>
       <c r="AF31" s="11">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="E32" s="11">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="G32" s="11">
-        <v>31</v>
+        <v>61</v>
+      </c>
+      <c r="H32" s="11">
+        <v>1</v>
       </c>
       <c r="I32" s="11">
-        <v>275</v>
+        <v>35</v>
       </c>
       <c r="J32" s="11">
-        <v>284</v>
+        <v>42</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="N32" s="11" t="s">
         <v>249</v>
@@ -7668,249 +7680,99 @@
       <c r="O32" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="P32" s="11" t="s">
-        <v>281</v>
-      </c>
       <c r="Q32" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S32" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="T32" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="V32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="W32" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="X32" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z32" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="AA32" s="11">
-        <v>2</v>
-      </c>
-      <c r="AB32" s="11">
-        <v>3</v>
-      </c>
-      <c r="AC32" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF32" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="AG32" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH32" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL32" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="AM32" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN32" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="AO32" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="AQ32" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR32" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS32" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AT32" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="AU32" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="AV32" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="AW32" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX32" s="11" t="s">
-        <v>379</v>
+      <c r="R32" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF32" s="11">
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="E33" s="11">
         <v>2003</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="G33" s="11">
+        <v>503</v>
+      </c>
+      <c r="I33" s="11">
+        <v>59</v>
+      </c>
+      <c r="J33" s="11">
         <v>67</v>
       </c>
-      <c r="H33" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="I33" s="11">
-        <v>33</v>
-      </c>
-      <c r="J33" s="11">
-        <v>45</v>
-      </c>
       <c r="K33" s="11" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="N33" s="11" t="s">
         <v>249</v>
       </c>
       <c r="O33" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="P33" s="11" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="Q33" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S33" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="T33" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="U33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V33" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="W33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X33" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z33" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="AA33" s="11">
-        <v>3</v>
-      </c>
-      <c r="AB33" s="11">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="11">
-        <v>3</v>
+      <c r="R33" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="AF33" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AG33" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH33" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK33" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL33" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="AM33" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="AO33" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="AP33" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="AQ33" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR33" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="AS33" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="AU33" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="AV33" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW33" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="AX33" s="11" t="s">
-        <v>385</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>243</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E34" s="11">
         <v>2003</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G34" s="11">
-        <v>67</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>316</v>
+        <v>31</v>
       </c>
       <c r="I34" s="11">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="J34" s="11">
-        <v>45</v>
+        <v>284</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="N34" s="11" t="s">
         <v>249</v>
@@ -7919,85 +7781,335 @@
         <v>250</v>
       </c>
       <c r="P34" s="11" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
       <c r="Q34" s="11" t="s">
         <v>21</v>
       </c>
       <c r="S34" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="T34" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V34" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="X34" s="11" t="s">
-        <v>72</v>
+        <v>216</v>
       </c>
       <c r="Z34" s="11" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="AA34" s="11">
+        <v>2</v>
+      </c>
+      <c r="AB34" s="11">
         <v>3</v>
       </c>
-      <c r="AB34" s="11">
-        <v>1</v>
-      </c>
       <c r="AC34" s="11">
-        <v>3</v>
-      </c>
-      <c r="AF34" s="11">
-        <v>4.4000000000000004</v>
+        <v>2</v>
+      </c>
+      <c r="AF34" s="11" t="s">
+        <v>321</v>
       </c>
       <c r="AG34" s="11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AH34" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK34" s="11" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="AL34" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="AM34" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
+      </c>
+      <c r="AN34" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="AO34" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="AP34" s="11" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="AQ34" s="11" t="s">
         <v>164</v>
       </c>
       <c r="AR34" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS34" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT34" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="AU34" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV34" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AW34" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX34" s="11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2003</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G35" s="11">
+        <v>67</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="I35" s="11">
+        <v>33</v>
+      </c>
+      <c r="J35" s="11">
+        <v>45</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="O35" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S35" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="T35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V35" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X35" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z35" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="AA35" s="11">
+        <v>3</v>
+      </c>
+      <c r="AB35" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="11">
+        <v>3</v>
+      </c>
+      <c r="AF35" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AG35" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH35" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK35" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL35" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="AM35" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO35" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="AP35" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="AQ35" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR35" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="AS34" s="11" t="s">
+      <c r="AS35" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="AU34" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="AV34" s="11" t="s">
+      <c r="AU35" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="AV35" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AW34" s="11" t="s">
+      <c r="AW35" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX35" s="11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E36" s="11">
+        <v>2003</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G36" s="11">
+        <v>67</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="I36" s="11">
+        <v>33</v>
+      </c>
+      <c r="J36" s="11">
+        <v>45</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="O36" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S36" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="T36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U36" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V36" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W36" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X36" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z36" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="AA36" s="11">
+        <v>3</v>
+      </c>
+      <c r="AB36" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="11">
+        <v>3</v>
+      </c>
+      <c r="AF36" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AG36" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH36" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK36" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL36" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="AM36" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO36" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="AP36" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="AQ36" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR36" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS36" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU36" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="AV36" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW36" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="AX34" s="11" t="s">
-        <v>385</v>
+      <c r="AX36" s="11" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -8032,7 +8144,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\kjova\Downloads\[DataExtractionForm_WP4_Brown.xlsx]Validation'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AF3:AF34</xm:sqref>
+          <xm:sqref>AF3:AF36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
@@ -10118,12 +10230,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10241,15 +10350,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10271,16 +10390,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>